<commit_message>
make cahnge to save parse answer choices
</commit_message>
<xml_diff>
--- a/PerpetHealthCheckIntro.xlsx
+++ b/PerpetHealthCheckIntro.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10211"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10311"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ivanpro/Dropbox/Equal/github/typeform/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ivanpro/Dropbox/Equal/git-perdev-dev/equal-survey/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{82576928-6C90-A34F-B013-F2192001B1A9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F53FEEDC-CD38-C54B-B89E-28C895A8A105}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="68800" yWindow="540" windowWidth="21600" windowHeight="20400" xr2:uid="{898366AA-613E-A547-9ABE-3031ABE0E9AC}"/>
+    <workbookView xWindow="25820" yWindow="1140" windowWidth="41540" windowHeight="21780" xr2:uid="{898366AA-613E-A547-9ABE-3031ABE0E9AC}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="262" uniqueCount="193">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="262" uniqueCount="194">
   <si>
     <t>Question</t>
   </si>
@@ -2093,9 +2093,6 @@
     <t>Start Next Phase</t>
   </si>
   <si>
-    <t>SET (@foldEar)</t>
-  </si>
-  <si>
     <t>AnswerChoices</t>
   </si>
   <si>
@@ -2202,57 +2199,17 @@
     <t>SET (@gender)</t>
   </si>
   <si>
-    <t>SET (@weight)</t>
-  </si>
-  <si>
     <t>SET (@age)</t>
-  </si>
-  <si>
-    <t>SET(@snack)</t>
   </si>
   <si>
     <t>APICALL(https://api.equal.pet/sign-service/v1/disease?is_main=true&amp;limit=500)
 EXTRACT(data.content[*].(id,name))</t>
   </si>
   <si>
-    <t>SET (@name)</t>
-  </si>
-  <si>
-    <t>SET (@neutralization_code)</t>
-  </si>
-  <si>
-    <t>SET (@main_act_place_code)</t>
-  </si>
-  <si>
-    <t>SET(@body_form_code)</t>
-  </si>
-  <si>
-    <t>SET (@relationship_code)</t>
-  </si>
-  <si>
     <t>SET (@disease_id)</t>
   </si>
   <si>
-    <t>SET (@disease_treat_code)</t>
-  </si>
-  <si>
-    <t>SET (@appetite_change_code)</t>
-  </si>
-  <si>
-    <t>SET (@feed_amount_code)</t>
-  </si>
-  <si>
-    <t>SET (@drinking_amount_code)</t>
-  </si>
-  <si>
     <t>SET (@allergy_id[])</t>
-  </si>
-  <si>
-    <t>SET (@walk_code)</t>
-  </si>
-  <si>
-    <t>M: 남자아이
-F: 여자아이</t>
   </si>
   <si>
     <t>{@name}의 품종은 무엇인가요?</t>
@@ -2281,28 +2238,6 @@
 cat: 고양이</t>
   </si>
   <si>
-    <t>SET (@type)</t>
-  </si>
-  <si>
-    <t>0: 병원에 진단 및 처방에 따라 치료하고 있어요
-1: 병원에서 진단만 받았어요</t>
-  </si>
-  <si>
-    <t>0: 줄었어요
-1: 비슷해요
-2: 늘었어요</t>
-  </si>
-  <si>
-    <t>0: 평소보다 활기차졌거나, 특별히 변화하지 않았어요
-1: 평소보다 조금 기운이 없어보여요
-2: 눈에 띄게 기력이 없어요</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0: 네
-1: 아니오. 하지만 할 예정이에요
-2: 아니오. 앞으로도 계획이 없어요   </t>
-  </si>
-  <si>
     <t>APICALL(https://api.equal.pet/sign-service/v1/breeds?type={@type}&amp;limit=500)
 EXTRACT(data.content[*].(id, name))</t>
   </si>
@@ -2310,48 +2245,10 @@
     <t>Multichoice - Single - Vertical</t>
   </si>
   <si>
-    <t>0: 하루 1번
-1: 하루 2번
-2: 하루 3번 이상
-3: 매일 하지는 않아요</t>
-  </si>
-  <si>
-    <t>0: 아니요.
-1: 네, 2마리가 함께 살고 있어요.
-2: 네, 3마리 이상이 함께 살고 있어요.</t>
-  </si>
-  <si>
-    <t>0: 실내 - 아파트, 빌라
-1: 실내 - 마당 있는 주택
-2: 실외 - 분리 거주 (마당 등)
-3: 실내 - 마당 있는 주택</t>
-  </si>
-  <si>
-    <t>0: 병원에서 진단을 받았어요.
-1: 병원에서 진단받은 적은 없지만, 의심되는 상황이 있었어요.</t>
-  </si>
-  <si>
     <t>APICALL(https://api.equal.pet/sign-service/v1/allergy?limit=500)
 EXTRACT(data.content[*].(id, name))</t>
   </si>
   <si>
-    <t>0: 동물병원 추천 또는 포장지에 적힌 정량만 줘요
-1: 동물병원 추천 또는 포장지에 적힌 정량보다 더 줘요
-2: 체중 감량이 필요하지는 않지만 동물병원 추천 또는 포장지에 적힌 정량보다 덜 줘요
-3: 체중 감량이 필요한 것 같아서 일부러 적게 주고 있어요
-4: 정량은 잘 모르지만 대략 정해서 주고 있어요
-5: 혼자 양을 조절해서 먹기 때문에 다 먹으면 채우고 있어서 잘 모르겠어요</t>
-  </si>
-  <si>
-    <t>0: 물을 잘 마시지 않는 것 같아요. 물그릇에 담긴 물이 잘 줄어들지 않아요
-1: 물그릇에 있는 물을 잘 마시지만, 추가로 더 달라고 조르지는 않아요
-2: 물그릇에 있는 물을 다 마시고, 부족하면 더 달라고 졸라요
-3: 과하다 싶을 정도로 계속 물을 달라고 졸라요</t>
-  </si>
-  <si>
-    <t>SET (@conditions_code)</t>
-  </si>
-  <si>
     <t>Y: 네
 N: 아니요</t>
   </si>
@@ -2365,22 +2262,129 @@
     <t>알레르기 성택해주세요 (중복 선택 가능)</t>
   </si>
   <si>
-    <t>SET (@how_to_know_allergy_code)
-IF (@type==dog) THEN (GOTO: 21) ELSE (GOTO: 24)</t>
-  </si>
-  <si>
     <t>IF (#Y) THEN (GOTO: 11) ELSE (GOTO: 13)</t>
-  </si>
-  <si>
-    <t>0: 저체중 - 많이 말랐어요 - IF(@type==cat) THEN IMG(bsc_cat01.imageset/bsc_cat01.png) ELSE IMG(bsc_dog01.imageset/bsc_dog01.png)
-1: 약간 저체중 - 마른 편이에요 - IF(@type==cat) THEN IMG(bsc_cat02.imageset/bsc_cat02.png) ELSE IMG(bsc_dog02.imageset/bsc_dog02.png)
-2 : 정상 - 딱 보기 좋아요 - IF(@type==cat) THEN IMG(bsc_cat03.imageset/bsc_cat03.png) ELSE IMG(bsc_dog03.imageset/bsc_dog03.png)
-3 : 준비만 - 조금 통통해요 - IF(@type==cat) THEN IMG(bsc_cat04.imageset/bsc_cat04.png) ELSE IMG(bsc_dog04.imageset/bsc_dog04.png)
-4 : 고도비만 - 뚱뚱해요 - IF(@type==cat) THEN IMG(bsc_cat05.imageset/bsc_cat05.png) ELSE IMG(bsc_dog05.imageset/bsc_dog05.png)</t>
   </si>
   <si>
     <t>IF (#Y) THEN (GOTO: 19)
 IF (@type==dog) THEN (GOTO: 21) ELSE (GOTO: 24)</t>
+  </si>
+  <si>
+    <t>SET (@pet_type)</t>
+  </si>
+  <si>
+    <t>SET (@pet_name)</t>
+  </si>
+  <si>
+    <t>SET (@body_weight)</t>
+  </si>
+  <si>
+    <t>SET (@neutering_surgery)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">performed: 네
+planned: 아니오. 하지만 할 예정이에요
+not_planned: 아니오. 앞으로도 계획이 없어요   </t>
+  </si>
+  <si>
+    <t>SET(@body_shape)</t>
+  </si>
+  <si>
+    <t>underweight_severe: 저체중 - 많이 말랐어요 - IF(@type==cat) THEN IMG(bsc_cat01.imageset/bsc_cat01.png) ELSE IMG(bsc_dog01.imageset/bsc_dog01.png)
+underweight_slight: 약간 저체중 - 마른 편이에요 - IF(@type==cat) THEN IMG(bsc_cat02.imageset/bsc_cat02.png) ELSE IMG(bsc_dog02.imageset/bsc_dog02.png)
+normal: 정상 - 딱 보기 좋아요 - IF(@type==cat) THEN IMG(bsc_cat03.imageset/bsc_cat03.png) ELSE IMG(bsc_dog03.imageset/bsc_dog03.png)
+overweight_slight : 준비만 - 조금 통통해요 - IF(@type==cat) THEN IMG(bsc_cat04.imageset/bsc_cat04.png) ELSE IMG(bsc_dog04.imageset/bsc_dog04.png)
+obese_severe: 고도비만 - 뚱뚱해요 - IF(@type==cat) THEN IMG(bsc_cat05.imageset/bsc_cat05.png) ELSE IMG(bsc_dog05.imageset/bsc_dog05.png)</t>
+  </si>
+  <si>
+    <t>SET (@energetic)</t>
+  </si>
+  <si>
+    <t>stable: 평소보다 활기차졌거나, 특별히 변화하지 않았어요
+slightly_decreased: 평소보다 조금 기운이 없어보여요
+significantly_decreased: 눈에 띄게 기력이 없어요</t>
+  </si>
+  <si>
+    <t>SET (@appetite)</t>
+  </si>
+  <si>
+    <t>decreased: 줄었어요
+unchanged: 비슷해요
+increased: 늘었어요</t>
+  </si>
+  <si>
+    <t>SET (@pet_food)</t>
+  </si>
+  <si>
+    <t>recommended_amount: 동물병원 추천 또는 포장지에 적힌 정량만 줘요
+more_than_recommended: 동물병원 추천 또는 포장지에 적힌 정량보다 더 줘요
+less_than_recommended: 체중 감량이 필요하지는 않지만 동물병원 추천 또는 포장지에 적힌 정량보다 덜 줘요
+less_for_weight_loss: 체중 감량이 필요한 것 같아서 일부러 적게 주고 있어요
+approximate_amount: 정량은 잘 모르지만 대략 정해서 주고 있어요
+self_regulated: 혼자 양을 조절해서 먹기 때문에 다 먹으면 채우고 있어서 잘 모르겠어요</t>
+  </si>
+  <si>
+    <t>SET(@treat)</t>
+  </si>
+  <si>
+    <t>yes: 네
+no: 아니요</t>
+  </si>
+  <si>
+    <t>SET (@water_intake)</t>
+  </si>
+  <si>
+    <t>low: 물을 잘 마시지 않는 것 같아요. 물그릇에 담긴 물이 잘 줄어들지 않아요
+normal: 물그릇에 있는 물을 잘 마시지만, 추가로 더 달라고 조르지는 않아요
+high: 물그릇에 있는 물을 다 마시고, 부족하면 더 달라고 졸라요
+excessive: 과하다 싶을 정도로 계속 물을 달라고 졸라요</t>
+  </si>
+  <si>
+    <t>diagnosed: 병원에서 진단을 받았어요.
+suspected: 병원에서 진단받은 적은 없지만, 의심되는 상황이 있었어요.</t>
+  </si>
+  <si>
+    <t>SET (@allergy_detect)
+IF (@type==dog) THEN (GOTO: 21) ELSE (GOTO: 24)</t>
+  </si>
+  <si>
+    <t>SET (@multi_animal_environment)</t>
+  </si>
+  <si>
+    <t>no: 아니요.
+two_animal: 네, 2마리가 함께 살고 있어요.
+more_than_three_animal: 네, 3마리 이상이 함께 살고 있어요.</t>
+  </si>
+  <si>
+    <t>SET (@living_space)</t>
+  </si>
+  <si>
+    <t>indoor_apartment: 실내 - 아파트, 빌라
+indoor_with_yard: 실내 - 마당 있는 주택
+indoor_without_yard: 실외 - 분리 거주 (마당 등)
+outdoor: 실내 - 마당 있는 주택</t>
+  </si>
+  <si>
+    <t>SET (@daily_walk)</t>
+  </si>
+  <si>
+    <t>once_a_day: 하루 1번
+twice_a_day: 하루 2번
+more_than_three_times_a_day: 하루 3번 이상
+not_every_day: 매일 하지는 않아요</t>
+  </si>
+  <si>
+    <t>SET (@ear_folded)</t>
+  </si>
+  <si>
+    <t>SET (@disease_treatment)</t>
+  </si>
+  <si>
+    <t>ongoing: 병원에 진단 및 처방에 따라 치료하고 있어요
+diagnosed_only: 병원에서 진단만 받았어요</t>
+  </si>
+  <si>
+    <t>male: 남자아이
+female: 여자아이</t>
   </si>
 </sst>
 </file>
@@ -2856,17 +2860,17 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4111223A-4AF6-0544-BC83-76B81098946D}">
   <dimension ref="A1:I85"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="124" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A7" zoomScaleNormal="124" workbookViewId="0">
       <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="4" customWidth="1"/>
-    <col min="2" max="2" width="40.83203125" customWidth="1"/>
+    <col min="2" max="2" width="38.33203125" customWidth="1"/>
     <col min="3" max="3" width="26.83203125" customWidth="1"/>
-    <col min="4" max="4" width="88.33203125" customWidth="1"/>
-    <col min="5" max="5" width="49.5" customWidth="1"/>
+    <col min="4" max="4" width="126.5" customWidth="1"/>
+    <col min="5" max="5" width="35.6640625" customWidth="1"/>
     <col min="6" max="6" width="55.83203125" customWidth="1"/>
     <col min="7" max="7" width="15.83203125" customWidth="1"/>
     <col min="8" max="8" width="26.83203125" customWidth="1"/>
@@ -2885,13 +2889,13 @@
         <v>13</v>
       </c>
       <c r="D1" s="3" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="E1" s="3" t="s">
         <v>3</v>
       </c>
       <c r="F1" s="3" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="G1" s="3" t="s">
         <v>4</v>
@@ -2905,13 +2909,13 @@
         <v>15</v>
       </c>
       <c r="C2" s="5" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="D2" s="5" t="s">
-        <v>169</v>
+        <v>155</v>
       </c>
       <c r="E2" s="20" t="s">
-        <v>170</v>
+        <v>165</v>
       </c>
       <c r="F2" s="5"/>
       <c r="G2" s="4" t="s">
@@ -2930,7 +2934,7 @@
       </c>
       <c r="D3" s="5"/>
       <c r="E3" s="5" t="s">
-        <v>149</v>
+        <v>166</v>
       </c>
       <c r="F3" s="5"/>
       <c r="G3" s="5"/>
@@ -2943,16 +2947,16 @@
         <v>53</v>
       </c>
       <c r="C4" s="5" t="s">
+        <v>135</v>
+      </c>
+      <c r="D4" s="5" t="s">
         <v>136</v>
       </c>
-      <c r="D4" s="5" t="s">
-        <v>137</v>
-      </c>
       <c r="E4" s="5" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="F4" s="5" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="G4" s="4"/>
     </row>
@@ -2961,19 +2965,19 @@
         <v>4</v>
       </c>
       <c r="B5" s="19" t="s">
-        <v>163</v>
+        <v>149</v>
       </c>
       <c r="C5" s="5" t="s">
         <v>2</v>
       </c>
       <c r="D5" s="5" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="E5" s="5" t="s">
-        <v>145</v>
+        <v>167</v>
       </c>
       <c r="F5" s="5" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="G5" s="4"/>
     </row>
@@ -2982,16 +2986,16 @@
         <v>5</v>
       </c>
       <c r="B6" s="19" t="s">
-        <v>162</v>
+        <v>148</v>
       </c>
       <c r="C6" s="5" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="D6" s="5" t="s">
-        <v>175</v>
+        <v>156</v>
       </c>
       <c r="E6" s="5" t="s">
-        <v>168</v>
+        <v>154</v>
       </c>
       <c r="F6" s="5" t="s">
         <v>6</v>
@@ -3003,19 +3007,19 @@
         <v>6</v>
       </c>
       <c r="B7" s="5" t="s">
-        <v>164</v>
+        <v>150</v>
       </c>
       <c r="C7" s="5" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="D7" s="20" t="s">
-        <v>185</v>
+        <v>179</v>
       </c>
       <c r="E7" s="5" t="s">
-        <v>110</v>
+        <v>190</v>
       </c>
       <c r="F7" s="5" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="G7" s="4" t="s">
         <v>6</v>
@@ -3026,19 +3030,19 @@
         <v>7</v>
       </c>
       <c r="B8" s="19" t="s">
-        <v>165</v>
+        <v>151</v>
       </c>
       <c r="C8" s="5" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="D8" s="5" t="s">
-        <v>161</v>
+        <v>193</v>
       </c>
       <c r="E8" s="5" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="F8" s="5" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="G8" s="6"/>
     </row>
@@ -3050,37 +3054,37 @@
         <v>62</v>
       </c>
       <c r="C9" s="5" t="s">
-        <v>176</v>
+        <v>157</v>
       </c>
       <c r="D9" s="5" t="s">
-        <v>174</v>
+        <v>169</v>
       </c>
       <c r="E9" s="5" t="s">
-        <v>150</v>
+        <v>168</v>
       </c>
       <c r="F9" s="5" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="G9" s="6"/>
     </row>
-    <row r="10" spans="1:7" ht="175" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:7" ht="137" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="4">
         <v>9</v>
       </c>
       <c r="B10" s="19" t="s">
-        <v>166</v>
+        <v>152</v>
       </c>
       <c r="C10" s="5" t="s">
+        <v>141</v>
+      </c>
+      <c r="D10" s="5" t="s">
+        <v>171</v>
+      </c>
+      <c r="E10" s="5" t="s">
+        <v>170</v>
+      </c>
+      <c r="F10" s="5" t="s">
         <v>142</v>
-      </c>
-      <c r="D10" s="5" t="s">
-        <v>191</v>
-      </c>
-      <c r="E10" s="5" t="s">
-        <v>152</v>
-      </c>
-      <c r="F10" s="5" t="s">
-        <v>143</v>
       </c>
       <c r="G10" s="6"/>
     </row>
@@ -3089,16 +3093,16 @@
         <v>10</v>
       </c>
       <c r="B11" s="5" t="s">
-        <v>187</v>
+        <v>161</v>
       </c>
       <c r="C11" s="5" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="D11" s="5" t="s">
-        <v>185</v>
+        <v>159</v>
       </c>
       <c r="E11" s="5" t="s">
-        <v>190</v>
+        <v>163</v>
       </c>
       <c r="F11" s="5"/>
       <c r="G11" s="6"/>
@@ -3108,16 +3112,16 @@
         <v>11</v>
       </c>
       <c r="B12" s="5" t="s">
-        <v>186</v>
+        <v>160</v>
       </c>
       <c r="C12" s="5" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="D12" s="5" t="s">
-        <v>148</v>
+        <v>145</v>
       </c>
       <c r="E12" s="5" t="s">
-        <v>154</v>
+        <v>146</v>
       </c>
       <c r="F12" s="5"/>
       <c r="G12" s="6"/>
@@ -3130,20 +3134,20 @@
         <v>75</v>
       </c>
       <c r="C13" s="5" t="s">
-        <v>176</v>
+        <v>157</v>
       </c>
       <c r="D13" s="5" t="s">
-        <v>171</v>
+        <v>192</v>
       </c>
       <c r="E13" s="5" t="s">
-        <v>155</v>
+        <v>191</v>
       </c>
       <c r="F13" s="5" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="G13" s="6"/>
     </row>
-    <row r="14" spans="1:7" ht="57" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:7" ht="60" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A14" s="4">
         <v>13</v>
       </c>
@@ -3151,16 +3155,16 @@
         <v>77</v>
       </c>
       <c r="C14" s="5" t="s">
-        <v>176</v>
+        <v>157</v>
       </c>
       <c r="D14" s="5" t="s">
         <v>173</v>
       </c>
       <c r="E14" s="5" t="s">
-        <v>184</v>
+        <v>172</v>
       </c>
       <c r="F14" s="5" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="G14" s="6"/>
     </row>
@@ -3172,37 +3176,37 @@
         <v>79</v>
       </c>
       <c r="C15" s="5" t="s">
-        <v>176</v>
+        <v>157</v>
       </c>
       <c r="D15" s="5" t="s">
-        <v>172</v>
+        <v>175</v>
       </c>
       <c r="E15" s="5" t="s">
-        <v>156</v>
+        <v>174</v>
       </c>
       <c r="F15" s="5" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="G15" s="4"/>
     </row>
-    <row r="16" spans="1:7" ht="118" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:7" ht="99" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A16" s="4">
         <v>15</v>
       </c>
       <c r="B16" s="19" t="s">
-        <v>167</v>
+        <v>153</v>
       </c>
       <c r="C16" s="5" t="s">
+        <v>157</v>
+      </c>
+      <c r="D16" s="5" t="s">
+        <v>177</v>
+      </c>
+      <c r="E16" s="5" t="s">
         <v>176</v>
       </c>
-      <c r="D16" s="5" t="s">
-        <v>182</v>
-      </c>
-      <c r="E16" s="5" t="s">
-        <v>157</v>
-      </c>
       <c r="F16" s="5" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="G16" s="4"/>
     </row>
@@ -3214,16 +3218,16 @@
         <v>81</v>
       </c>
       <c r="C17" s="5" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="D17" s="20" t="s">
-        <v>185</v>
+        <v>179</v>
       </c>
       <c r="E17" s="5" t="s">
-        <v>147</v>
+        <v>178</v>
       </c>
       <c r="F17" s="5" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
     </row>
     <row r="18" spans="1:9" ht="71" customHeight="1" x14ac:dyDescent="0.2">
@@ -3234,16 +3238,16 @@
         <v>82</v>
       </c>
       <c r="C18" s="5" t="s">
-        <v>176</v>
+        <v>157</v>
       </c>
       <c r="D18" s="5" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="E18" s="5" t="s">
-        <v>158</v>
+        <v>180</v>
       </c>
       <c r="F18" s="5" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="G18" s="4"/>
     </row>
@@ -3255,13 +3259,13 @@
         <v>83</v>
       </c>
       <c r="C19" s="5" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="D19" s="5" t="s">
-        <v>185</v>
+        <v>159</v>
       </c>
       <c r="E19" s="5" t="s">
-        <v>192</v>
+        <v>164</v>
       </c>
       <c r="F19" s="4"/>
     </row>
@@ -3270,16 +3274,16 @@
         <v>19</v>
       </c>
       <c r="B20" s="5" t="s">
-        <v>188</v>
+        <v>162</v>
       </c>
       <c r="C20" s="5" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="D20" s="5" t="s">
-        <v>181</v>
+        <v>158</v>
       </c>
       <c r="E20" s="5" t="s">
-        <v>159</v>
+        <v>147</v>
       </c>
       <c r="F20" s="4"/>
     </row>
@@ -3291,16 +3295,16 @@
         <v>85</v>
       </c>
       <c r="C21" s="5" t="s">
-        <v>176</v>
+        <v>157</v>
       </c>
       <c r="D21" s="5" t="s">
-        <v>180</v>
+        <v>182</v>
       </c>
       <c r="E21" s="5" t="s">
-        <v>189</v>
+        <v>183</v>
       </c>
       <c r="F21" s="5" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="G21" s="4"/>
     </row>
@@ -3312,16 +3316,16 @@
         <v>84</v>
       </c>
       <c r="C22" s="5" t="s">
-        <v>176</v>
+        <v>157</v>
       </c>
       <c r="D22" s="5" t="s">
-        <v>177</v>
+        <v>189</v>
       </c>
       <c r="E22" s="5" t="s">
-        <v>160</v>
+        <v>188</v>
       </c>
       <c r="F22" s="5" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="G22" s="4"/>
     </row>
@@ -3333,16 +3337,16 @@
         <v>86</v>
       </c>
       <c r="C23" s="5" t="s">
-        <v>176</v>
+        <v>157</v>
       </c>
       <c r="D23" s="5" t="s">
-        <v>178</v>
+        <v>185</v>
       </c>
       <c r="E23" s="5" t="s">
-        <v>153</v>
+        <v>184</v>
       </c>
       <c r="F23" s="5" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="G23" s="6"/>
     </row>
@@ -3354,16 +3358,16 @@
         <v>87</v>
       </c>
       <c r="C24" s="5" t="s">
-        <v>176</v>
+        <v>157</v>
       </c>
       <c r="D24" s="5" t="s">
-        <v>179</v>
+        <v>187</v>
       </c>
       <c r="E24" s="5" t="s">
-        <v>151</v>
+        <v>186</v>
       </c>
       <c r="F24" s="5" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="G24" s="4"/>
     </row>
@@ -3381,7 +3385,7 @@
         <v>109</v>
       </c>
       <c r="E25" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="F25" s="5"/>
       <c r="G25" s="1"/>
@@ -3665,7 +3669,7 @@
         <v>16</v>
       </c>
       <c r="E2" s="5" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="F2" s="4" t="s">
         <v>6</v>
@@ -3730,7 +3734,7 @@
         <v>1</v>
       </c>
       <c r="D6" s="14" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="E6" s="14" t="s">
         <v>56</v>
@@ -3750,7 +3754,7 @@
         <v>10</v>
       </c>
       <c r="D7" s="5" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="E7" s="5" t="s">
         <v>59</v>
@@ -3806,7 +3810,7 @@
         <v>70</v>
       </c>
       <c r="D10" s="17" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="E10" s="17" t="s">
         <v>63</v>
@@ -3824,7 +3828,7 @@
         <v>73</v>
       </c>
       <c r="D11" s="14" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="E11" s="14" t="s">
         <v>71</v>
@@ -3946,7 +3950,7 @@
       </c>
       <c r="C18" s="14"/>
       <c r="D18" s="14" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="E18" s="14" t="s">
         <v>98</v>

</xml_diff>